<commit_message>
Save Excel to DB
</commit_message>
<xml_diff>
--- a/EasyPro/wwwroot/UploadExcel/Employees.xlsx
+++ b/EasyPro/wwwroot/UploadExcel/Employees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DB5B0FC-E31A-4B3F-89AD-821738004EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7839BA73-6A86-49A5-8DF5-EAB3DD7E5046}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="employee" sheetId="1" r:id="rId1"/>
@@ -32,57 +32,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t>EmployeeId</t>
+    <t>Milk</t>
   </si>
   <si>
-    <t>EmployeeName</t>
+    <t>Qnty</t>
   </si>
   <si>
-    <t>Age</t>
+    <t>Product</t>
   </si>
   <si>
-    <t>Sex</t>
+    <t>Sno</t>
   </si>
   <si>
-    <t>Designation</t>
-  </si>
-  <si>
-    <t>Jack Supreu</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Solution Architect</t>
-  </si>
-  <si>
-    <t>Steve khan</t>
-  </si>
-  <si>
-    <t>Software Engineer</t>
-  </si>
-  <si>
-    <t>Romi gill</t>
-  </si>
-  <si>
-    <t>FeMale</t>
-  </si>
-  <si>
-    <t>Junior Consultant</t>
-  </si>
-  <si>
-    <t>Hider Ali</t>
-  </si>
-  <si>
-    <t>Accountant</t>
-  </si>
-  <si>
-    <t>Mathew</t>
-  </si>
-  <si>
-    <t>Human Resource</t>
+    <t>TransDate</t>
   </si>
 </sst>
 </file>
@@ -118,8 +82,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,117 +399,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>45</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44568</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6">
-        <v>48</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
+      <c r="D3" s="1">
+        <v>44599</v>
       </c>
     </row>
   </sheetData>

</xml_diff>